<commit_message>
Changement + Test IHM
Quelques changements dans les requirements et ajout des test sur les
requirements de l'IHM
</commit_message>
<xml_diff>
--- a/Requirement  Projet JEE.xlsx
+++ b/Requirement  Projet JEE.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Requirement" sheetId="1" r:id="rId1"/>
+    <sheet name="Test IHM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -289,13 +290,64 @@
   </si>
   <si>
     <t>L'IHM doit contenir un bouton "Connect" permettant la connection si les login et mot de passe entrés sont valides</t>
+  </si>
+  <si>
+    <t>APP_SERVER_008</t>
+  </si>
+  <si>
+    <t>L'utilisateur peut envoyer un message tapé en appuyant sur la touche entrée</t>
+  </si>
+  <si>
+    <t>APP_IHM_008</t>
+  </si>
+  <si>
+    <t>Le serveur accepte un nombre illimité de connexions de client simultanément</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test to be made </t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Check on the source code the location of the classes in the project</t>
+  </si>
+  <si>
+    <t>Launch the IHM, an authentification window must be the first page</t>
+  </si>
+  <si>
+    <t>Launch the IHM, an option for administrator authentification must be present on the first page</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>After successful login, a chat field must be present</t>
+  </si>
+  <si>
+    <t>Launch the IHM, a "Connect" button must be present to send the authentification request to the server</t>
+  </si>
+  <si>
+    <t>After successful login, a "Send" button must be present to send the user's message to the server</t>
+  </si>
+  <si>
+    <t>O / M ?</t>
+  </si>
+  <si>
+    <t>After succesfful login, write a message and push the "Enter" key. The message must be send to the server</t>
+  </si>
+  <si>
+    <t>Try to log in with and existing nickname. The system must send an error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,8 +380,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +456,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -446,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -503,6 +569,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -824,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:G40"/>
+  <dimension ref="D2:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,63 +1161,63 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D22" s="18"/>
       <c r="E22" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D23" s="18"/>
+      <c r="E23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="19" t="s">
+      <c r="G23" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D24" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="19"/>
-      <c r="E24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>85</v>
-      </c>
       <c r="G24" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" s="19"/>
       <c r="E25" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D26" s="19"/>
       <c r="E26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>5</v>
@@ -1148,7 +1226,7 @@
     <row r="27" spans="4:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D27" s="19"/>
       <c r="E27" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>87</v>
@@ -1157,63 +1235,63 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="4:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D28" s="19"/>
       <c r="E28" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:7" ht="45" x14ac:dyDescent="0.25">
       <c r="D29" s="19"/>
       <c r="E29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D30" s="19"/>
+      <c r="E30" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F30" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="19"/>
+      <c r="E31" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="15" t="s">
+      <c r="G31" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D32" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="15"/>
-      <c r="E31" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D32" s="15"/>
-      <c r="E32" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>5</v>
@@ -1222,10 +1300,10 @@
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" s="15"/>
       <c r="E33" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>5</v>
@@ -1233,11 +1311,11 @@
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34" s="15"/>
-      <c r="E34" s="9" t="s">
-        <v>55</v>
+      <c r="E34" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>5</v>
@@ -1245,11 +1323,11 @@
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D35" s="15"/>
-      <c r="E35" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>52</v>
+      <c r="E35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>5</v>
@@ -1258,76 +1336,273 @@
     <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D36" s="15"/>
       <c r="E36" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D37" s="15"/>
       <c r="E37" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D38" s="15"/>
+      <c r="E38" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D39" s="15"/>
+      <c r="E39" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D38" s="16" t="s">
+      <c r="G39" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="4:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D40" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E40" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F40" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D39" s="16"/>
-      <c r="E39" s="10" t="s">
+      <c r="G40" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D41" s="16"/>
+      <c r="E41" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F41" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G39" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D40" s="13" t="s">
+      <c r="G41" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D42" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E42" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="F42" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="G42" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="D7:D14"/>
-    <mergeCell ref="D30:D37"/>
-    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D32:D39"/>
+    <mergeCell ref="D40:D41"/>
     <mergeCell ref="D3:D6"/>
-    <mergeCell ref="D15:D22"/>
-    <mergeCell ref="D23:D29"/>
+    <mergeCell ref="D15:D23"/>
+    <mergeCell ref="D24:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="56.140625" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="str">
+        <f>Requirement!E24</f>
+        <v>APP_IHM_001</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f>Requirement!G24</f>
+        <v>Mandatory</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="str">
+        <f>Requirement!E25</f>
+        <v>APP_IHM_002</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f>Requirement!G25</f>
+        <v>Mandatory</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="str">
+        <f>Requirement!E26</f>
+        <v>APP_IHM_003</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f>Requirement!G26</f>
+        <v>Mandatory</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="str">
+        <f>Requirement!E27</f>
+        <v>APP_IHM_004</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f>Requirement!G27</f>
+        <v>Mandatory</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="str">
+        <f>Requirement!E28</f>
+        <v>APP_IHM_005</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f>Requirement!G28</f>
+        <v>Mandatory</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="str">
+        <f>Requirement!E29</f>
+        <v>APP_IHM_006</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f>Requirement!G29</f>
+        <v>Mandatory</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="str">
+        <f>Requirement!E30</f>
+        <v>APP_IHM_007</v>
+      </c>
+      <c r="C9" s="20" t="str">
+        <f>Requirement!G30</f>
+        <v>Optionnal</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="str">
+        <f>Requirement!E31</f>
+        <v>APP_IHM_008</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f>Requirement!G31</f>
+        <v>Mandatory</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add FRT, PMP and DIR
</commit_message>
<xml_diff>
--- a/Requirement  Projet JEE.xlsx
+++ b/Requirement  Projet JEE.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morea\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thibault\Documents\GitHub\PROJET_JEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,8 +16,7 @@
     <sheet name="Test IHM" sheetId="2" r:id="rId2"/>
     <sheet name="Test Bug" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="122">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -382,12 +381,24 @@
   </si>
   <si>
     <t>Le client doit envoyer un "KeepAlive" toutes les secondes afin d'éviter toute déconnexion</t>
+  </si>
+  <si>
+    <t>APP_JAVA_005</t>
+  </si>
+  <si>
+    <t>L'application sera un jar exécutable</t>
+  </si>
+  <si>
+    <t>APP_JAVA_006</t>
+  </si>
+  <si>
+    <t>L'application se lancera avec un bat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -646,25 +657,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -986,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G48"/>
+  <dimension ref="A2:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,10 +1030,10 @@
         <v>116</v>
       </c>
       <c r="B3" s="12">
-        <f>COUNTA(E3:E140)</f>
-        <v>45</v>
-      </c>
-      <c r="D3" s="22" t="s">
+        <f>COUNTA(E3:E142)</f>
+        <v>47</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="19" t="s">
@@ -1036,7 +1047,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="22"/>
+      <c r="D4" s="27"/>
       <c r="E4" s="19" t="s">
         <v>27</v>
       </c>
@@ -1048,7 +1059,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="22"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="19" t="s">
         <v>28</v>
       </c>
@@ -1060,258 +1071,256 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="22"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="19" t="s">
         <v>75</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="27"/>
+      <c r="E7" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="27"/>
+      <c r="E8" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="23" t="s">
+      <c r="G8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="23"/>
-      <c r="E8" s="19" t="s">
+      <c r="G9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="26"/>
+      <c r="E10" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="23"/>
-      <c r="E9" s="19" t="s">
+      <c r="G10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="26"/>
+      <c r="E11" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="23"/>
-      <c r="E10" s="19" t="s">
+      <c r="G11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="26"/>
+      <c r="E12" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="23"/>
-      <c r="E11" s="19" t="s">
+      <c r="G12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="26"/>
+      <c r="E13" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="23"/>
-      <c r="E12" s="19" t="s">
+      <c r="G13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="26"/>
+      <c r="E14" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="23"/>
-      <c r="E13" s="19" t="s">
+      <c r="G14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="26"/>
+      <c r="E15" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="23"/>
-      <c r="E14" s="19" t="s">
+    <row r="16" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="26"/>
+      <c r="E16" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="23"/>
-      <c r="E15" s="19" t="s">
+      <c r="G16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="26"/>
+      <c r="E17" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="23"/>
-      <c r="E16" s="19" t="s">
+      <c r="G17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="26"/>
+      <c r="E18" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="24" t="s">
+      <c r="G18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E19" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="24"/>
-      <c r="E18" s="19" t="s">
+      <c r="G19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="25"/>
+      <c r="E20" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="24"/>
-      <c r="E19" s="19" t="s">
+      <c r="G20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="25"/>
+      <c r="E21" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G21" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="24"/>
-      <c r="E20" s="19" t="s">
+    <row r="22" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="25"/>
+      <c r="E22" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="24"/>
-      <c r="E21" s="19" t="s">
+      <c r="G22" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="25"/>
+      <c r="E23" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="24"/>
-      <c r="E22" s="19" t="s">
+      <c r="G23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="25"/>
+      <c r="E24" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F24" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="24"/>
-      <c r="E23" s="19" t="s">
+      <c r="G24" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="25"/>
+      <c r="E25" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="24"/>
-      <c r="E24" s="19" t="s">
+      <c r="G25" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="25"/>
+      <c r="E26" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F26" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="24"/>
-      <c r="E25" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>4</v>
@@ -1320,270 +1329,296 @@
     <row r="27" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="25"/>
       <c r="E27" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="24"/>
+      <c r="E29" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F29" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="25"/>
-      <c r="E28" s="19" t="s">
+      <c r="G29" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="24"/>
+      <c r="E30" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F30" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="25"/>
-      <c r="E29" s="19" t="s">
+      <c r="G30" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="24"/>
+      <c r="E31" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F31" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="25"/>
-      <c r="E30" s="19" t="s">
+      <c r="G31" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="24"/>
+      <c r="E32" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="4:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="25"/>
-      <c r="E31" s="19" t="s">
+      <c r="G32" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="24"/>
+      <c r="E33" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="25"/>
-      <c r="E32" s="19" t="s">
+      <c r="G33" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="24"/>
+      <c r="E34" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G34" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="25"/>
-      <c r="E33" s="19" t="s">
+    <row r="35" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="24"/>
+      <c r="E35" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F35" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="26" t="s">
+      <c r="G35" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="E36" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F36" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="26"/>
-      <c r="E35" s="19" t="s">
+      <c r="G36" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="28"/>
+      <c r="E37" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F37" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="26"/>
-      <c r="E36" s="19" t="s">
+      <c r="G37" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="28"/>
+      <c r="E38" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F38" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="26"/>
-      <c r="E37" s="19" t="s">
+      <c r="G38" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="28"/>
+      <c r="E39" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F39" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="26"/>
-      <c r="E38" s="19" t="s">
+      <c r="G39" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="28"/>
+      <c r="E40" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F40" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D39" s="26"/>
-      <c r="E39" s="19" t="s">
+      <c r="G40" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="28"/>
+      <c r="E41" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F41" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="26"/>
-      <c r="E40" s="20" t="s">
+      <c r="G41" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="28"/>
+      <c r="E42" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F42" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="26"/>
-      <c r="E41" s="20" t="s">
+      <c r="G42" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="28"/>
+      <c r="E43" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="26"/>
-      <c r="E42" s="20" t="s">
+      <c r="G43" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="28"/>
+      <c r="E44" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F44" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="26"/>
-      <c r="E43" s="20" t="s">
+      <c r="G44" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="28"/>
+      <c r="E45" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="F45" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="26"/>
-      <c r="E44" s="20" t="s">
+      <c r="G45" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="28"/>
+      <c r="E46" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F46" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="4:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="27" t="s">
+      <c r="G46" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="4:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D47" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="E45" s="20" t="s">
+      <c r="E47" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F47" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G45" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="27"/>
-      <c r="E46" s="21" t="s">
+      <c r="G47" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="4:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="23"/>
+      <c r="E48" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="F48" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G46" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="28" t="s">
+      <c r="G48" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D49" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="20" t="s">
+      <c r="E49" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F49" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="G49" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="4:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="4:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D26:D33"/>
-    <mergeCell ref="D17:D25"/>
-    <mergeCell ref="D7:D16"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="D34:D44"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D28:D35"/>
+    <mergeCell ref="D19:D27"/>
+    <mergeCell ref="D9:D18"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="D36:D46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1623,11 +1658,11 @@
     </row>
     <row r="3" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
-        <f>Requirement!E26</f>
+        <f>Requirement!E28</f>
         <v>APP_IHM_001</v>
       </c>
       <c r="C3" s="2" t="str">
-        <f>Requirement!G26</f>
+        <f>Requirement!G28</f>
         <v>Mandatory</v>
       </c>
       <c r="D3" s="14" t="s">
@@ -1640,11 +1675,11 @@
     </row>
     <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
-        <f>Requirement!E27</f>
+        <f>Requirement!E29</f>
         <v>APP_IHM_002</v>
       </c>
       <c r="C4" s="2" t="str">
-        <f>Requirement!G27</f>
+        <f>Requirement!G29</f>
         <v>Mandatory</v>
       </c>
       <c r="D4" s="14" t="s">
@@ -1657,11 +1692,11 @@
     </row>
     <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
-        <f>Requirement!E28</f>
+        <f>Requirement!E30</f>
         <v>APP_IHM_003</v>
       </c>
       <c r="C5" s="2" t="str">
-        <f>Requirement!G28</f>
+        <f>Requirement!G30</f>
         <v>Mandatory</v>
       </c>
       <c r="D5" s="14" t="s">
@@ -1674,11 +1709,11 @@
     </row>
     <row r="6" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
-        <f>Requirement!E29</f>
+        <f>Requirement!E31</f>
         <v>APP_IHM_004</v>
       </c>
       <c r="C6" s="2" t="str">
-        <f>Requirement!G29</f>
+        <f>Requirement!G31</f>
         <v>Mandatory</v>
       </c>
       <c r="D6" s="14" t="s">
@@ -1691,11 +1726,11 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
-        <f>Requirement!E30</f>
+        <f>Requirement!E32</f>
         <v>APP_IHM_005</v>
       </c>
       <c r="C7" s="2" t="str">
-        <f>Requirement!G30</f>
+        <f>Requirement!G32</f>
         <v>Mandatory</v>
       </c>
       <c r="D7" s="14" t="s">
@@ -1708,11 +1743,11 @@
     </row>
     <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
-        <f>Requirement!E31</f>
+        <f>Requirement!E33</f>
         <v>APP_IHM_006</v>
       </c>
       <c r="C8" s="2" t="str">
-        <f>Requirement!G31</f>
+        <f>Requirement!G33</f>
         <v>Mandatory</v>
       </c>
       <c r="D8" s="14" t="s">
@@ -1725,11 +1760,11 @@
     </row>
     <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
-        <f>Requirement!E32</f>
+        <f>Requirement!E34</f>
         <v>APP_IHM_007</v>
       </c>
       <c r="C9" s="11" t="str">
-        <f>Requirement!G32</f>
+        <f>Requirement!G34</f>
         <v>Optionnal</v>
       </c>
       <c r="D9" s="14" t="s">
@@ -1742,11 +1777,11 @@
     </row>
     <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="str">
-        <f>Requirement!E33</f>
+        <f>Requirement!E35</f>
         <v>APP_IHM_008</v>
       </c>
       <c r="C10" s="2" t="str">
-        <f>Requirement!G33</f>
+        <f>Requirement!G35</f>
         <v>Mandatory</v>
       </c>
       <c r="D10" s="14" t="s">

</xml_diff>